<commit_message>
Updated templates and main readme w.r.t. doc
</commit_message>
<xml_diff>
--- a/annotation tables/Simi Annotation Table Example.xlsx
+++ b/annotation tables/Simi Annotation Table Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahan/sciebo/PythonCode/AutoGaitA Docs &amp; Backups/SC XLS Doc Templates Examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahan/sciebo/PythonCode/autogaita_repository/annotation tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA820EA-09C7-E64B-91E5-4931B6583749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7E6ED0-EA5E-2044-A0EA-BEFB6701BB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15700" xr2:uid="{EDC322E6-FB3F-534D-BD9B-4E65E46A4375}"/>
+    <workbookView xWindow="38720" yWindow="500" windowWidth="29920" windowHeight="17220" xr2:uid="{EDC322E6-FB3F-534D-BD9B-4E65E46A4375}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9FB4BB-7540-014F-B48A-6F1B7CB0B23D}">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>